<commit_message>
Updated theme and readme
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/R_packages/mediocrethemes/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BD2C948-FCAE-1F4E-B0CA-B38E76F98598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4F923-80D8-3345-8184-03023D6D751C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15760" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -50,18 +50,12 @@
     <t>base</t>
   </si>
   <si>
-    <t>#283845</t>
-  </si>
-  <si>
     <t>#D9F8D1</t>
   </si>
   <si>
     <t>light</t>
   </si>
   <si>
-    <t>#4A6982</t>
-  </si>
-  <si>
     <t>background</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>#1D2834</t>
+  </si>
+  <si>
+    <t>#15343D</t>
+  </si>
+  <si>
+    <t>#1F4D5B</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:J10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,13 +445,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -462,13 +462,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -476,16 +476,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Color scale in execl document
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD95ED6F-C733-FD4C-9633-4DD569FD310B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E2A269-51B0-4248-B83F-6A6AC88A1663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15760" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>color</t>
   </si>
@@ -83,23 +83,35 @@
     <t>complementary</t>
   </si>
   <si>
-    <t>#6A3524</t>
-  </si>
-  <si>
     <t>#6B2E50</t>
+  </si>
+  <si>
+    <t>#81402C</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>#15343D, #284046, #3E4D4E, #5F5B4E, #856949, #AB7743, #D2863C, #FB9637, #E57630, #D0562B, #BC3626, #A61922, #8D0422, #70002A, #520036</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +478,11 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -483,10 +499,10 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -503,7 +519,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional color palette (rainbow)
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23D0AFF-E1C6-F64E-919E-50CE49101EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24896ECD-33F4-8A40-9C0A-3D73DE355A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15760" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,35 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>color</t>
   </si>
   <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>gray</t>
-  </si>
-  <si>
-    <t>#2D6A48</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
-    <t>#D9F8D1</t>
-  </si>
-  <si>
     <t>light</t>
   </si>
   <si>
     <t>background</t>
   </si>
   <si>
-    <t>#1C4221</t>
-  </si>
-  <si>
     <t>dark</t>
   </si>
   <si>
@@ -71,18 +56,12 @@
     <t>#1F4D5B</t>
   </si>
   <si>
-    <t>#FFFDF2</t>
-  </si>
-  <si>
     <t>#F9FAF7</t>
   </si>
   <si>
     <t>complementary</t>
   </si>
   <si>
-    <t>#6B2E50</t>
-  </si>
-  <si>
     <t>#81402C</t>
   </si>
   <si>
@@ -93,6 +72,36 @@
   </si>
   <si>
     <t>#00313C, #183C41, #304746, #48514A, #856949, #AB7743, #D2863C, #FB9637, #E57630, #D0562B, #BC3626, #A61922, #8D0422, #70002A, #520036</t>
+  </si>
+  <si>
+    <t>rainbow</t>
+  </si>
+  <si>
+    <t>#C65D44</t>
+  </si>
+  <si>
+    <t>autumn</t>
+  </si>
+  <si>
+    <t>#44ACC5</t>
+  </si>
+  <si>
+    <t>#652D1F</t>
+  </si>
+  <si>
+    <t>#1B3037, #213C47, #26525B, #28847D, #45A289, #7CAE7F, #B2B974, #E9C46A, #ECBA67, #EFB065, #F2A662, #F0935C, #E87653, #D8674B, #C65D44</t>
+  </si>
+  <si>
+    <t>#F4A261</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>#FCFAF7</t>
+  </si>
+  <si>
+    <t>#213C47</t>
   </si>
 </sst>
 </file>
@@ -451,78 +460,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding mediocre_xaringan (before checks)
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/R_packages/mediocrethemes/inst/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3772293F-D5E9-2342-8C2C-47273DA7E30F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213A308A-DE9A-8E49-A58F-F11715215205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>complementary</t>
   </si>
   <si>
-    <t>#81402C</t>
-  </si>
-  <si>
     <t>vector</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>#1D4749, #1C5659, #1C6669, #2E8481, #49AA9C, #6EC6B0, #A7D1B4, #E1DDB9, #E5C38A, #EAA95C, #E78541, #DF5D2F, #CF3E22, #AD341C, #8C2A17</t>
+  </si>
+  <si>
+    <t>#FB9637</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -587,18 +587,18 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -610,140 +610,140 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T%+replace% instead of + and corrected palettes
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213A308A-DE9A-8E49-A58F-F11715215205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5E0F7D-FA22-1549-901B-22C9F64EF15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>color</t>
   </si>
@@ -77,9 +77,6 @@
     <t>autumn</t>
   </si>
   <si>
-    <t>#44ACC5</t>
-  </si>
-  <si>
     <t>#652D1F</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>#D8F3DC, #C3E0C9, #AFCDB7, #9BBAA5, #87A793, #739480, #5E816E, #4A6E5C, #365C4A, #214938, #1A3F2F, #19392B, #183327, #172D23, #162720</t>
   </si>
   <si>
-    <t>#D8674B</t>
-  </si>
-  <si>
     <t>#1D3557</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>#0F1C2E</t>
   </si>
   <si>
-    <t>#AC7E39</t>
-  </si>
-  <si>
     <t>#1D3557, #2E5375, #3F7193, #6196AF, #8BBECA, #B0DDDC, #CAEADD, #E5F6DF, #E8CEC1, #EBA7A3, #EA7E82, #E7545D, #DF3643, #CB303C, #B72A35</t>
   </si>
   <si>
@@ -182,9 +173,6 @@
     <t>#E1DDB9</t>
   </si>
   <si>
-    <t>#EA9534</t>
-  </si>
-  <si>
     <t>#112A2C</t>
   </si>
   <si>
@@ -195,6 +183,9 @@
   </si>
   <si>
     <t>#FB9637</t>
+  </si>
+  <si>
+    <t>#1B3037</t>
   </si>
 </sst>
 </file>
@@ -556,7 +547,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -610,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -621,129 +612,129 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explicit colors when few categories
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5E0F7D-FA22-1549-901B-22C9F64EF15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB7B66-F39E-CD4D-960C-F28079446E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>color</t>
   </si>
@@ -186,6 +186,27 @@
   </si>
   <si>
     <t>#1B3037</t>
+  </si>
+  <si>
+    <t>four_colors</t>
+  </si>
+  <si>
+    <t>#1B3037, #E9C46A, #28847D, #C65D44</t>
+  </si>
+  <si>
+    <t>#162720, #87A793, #D8F3DC, #214938</t>
+  </si>
+  <si>
+    <t>#1D3557, #E8CEC1, #6196AF, #CB303C</t>
+  </si>
+  <si>
+    <t>#1C6669, #E5C38A, #E08E53, #913827</t>
+  </si>
+  <si>
+    <t>#00313C, #FB9637, #856949, #70002A</t>
+  </si>
+  <si>
+    <t>#1D1F20, #A6AAAD, #6F7274, #D0D4D7</t>
   </si>
 </sst>
 </file>
@@ -544,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,7 +576,7 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,8 +601,11 @@
       <c r="H1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -606,8 +630,11 @@
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -632,8 +659,11 @@
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -658,8 +688,11 @@
       <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -684,8 +717,11 @@
       <c r="H5" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -710,8 +746,12 @@
       <c r="H6" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -735,6 +775,9 @@
       </c>
       <c r="H7" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simpler handling of light colors
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB7B66-F39E-CD4D-960C-F28079446E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123EE61-3B2B-1F48-B32F-7BF4527277BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>color</t>
   </si>
@@ -41,21 +41,9 @@
     <t>base</t>
   </si>
   <si>
-    <t>light</t>
-  </si>
-  <si>
     <t>background</t>
   </si>
   <si>
-    <t>dark</t>
-  </si>
-  <si>
-    <t>#1D2834</t>
-  </si>
-  <si>
-    <t>#1F4D5B</t>
-  </si>
-  <si>
     <t>#F9FAF7</t>
   </si>
   <si>
@@ -77,15 +65,9 @@
     <t>autumn</t>
   </si>
   <si>
-    <t>#652D1F</t>
-  </si>
-  <si>
     <t>#1B3037, #213C47, #26525B, #28847D, #45A289, #7CAE7F, #B2B974, #E9C46A, #ECBA67, #EFB065, #F2A662, #F0935C, #E87653, #D8674B, #C65D44</t>
   </si>
   <si>
-    <t>#F4A261</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -104,12 +86,6 @@
     <t>#1B4332</t>
   </si>
   <si>
-    <t>#7A9B87</t>
-  </si>
-  <si>
-    <t>#0F1A15</t>
-  </si>
-  <si>
     <t>#6C2B46</t>
   </si>
   <si>
@@ -125,12 +101,6 @@
     <t>#14253E</t>
   </si>
   <si>
-    <t>#457B9D</t>
-  </si>
-  <si>
-    <t>#0F1C2E</t>
-  </si>
-  <si>
     <t>#1D3557, #2E5375, #3F7193, #6196AF, #8BBECA, #B0DDDC, #CAEADD, #E5F6DF, #E8CEC1, #EBA7A3, #EA7E82, #E7545D, #DF3643, #CB303C, #B72A35</t>
   </si>
   <si>
@@ -146,15 +116,9 @@
     <t>#F9FAFA</t>
   </si>
   <si>
-    <t>#1D1F20</t>
-  </si>
-  <si>
     <t>#212529</t>
   </si>
   <si>
-    <t>#CED4DA</t>
-  </si>
-  <si>
     <t>#6C757D</t>
   </si>
   <si>
@@ -168,12 +132,6 @@
   </si>
   <si>
     <t>#1D4749</t>
-  </si>
-  <si>
-    <t>#E1DDB9</t>
-  </si>
-  <si>
-    <t>#112A2C</t>
   </si>
   <si>
     <t>#F9F8F1</t>
@@ -565,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +534,7 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,200 +542,158 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>56</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding palettes: leo, portal, pem
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123EE61-3B2B-1F48-B32F-7BF4527277BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E905EB92-B5F6-9B4A-A33D-7F2C88342B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
+    <workbookView xWindow="1380" yWindow="560" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>color</t>
   </si>
@@ -165,6 +165,60 @@
   </si>
   <si>
     <t>#1D1F20, #A6AAAD, #6F7274, #D0D4D7</t>
+  </si>
+  <si>
+    <t>leo</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#FEFEF1</t>
+  </si>
+  <si>
+    <t>#0081A7</t>
+  </si>
+  <si>
+    <t>#004154, #00556F, #006D8D, #0087A9, #00A8B6, #48C5C3, #A2E0CF, #FDFCDC, #FDE3C1, #F8AC94, #EA6E64, #CC5F58, #994C47, #6D3C39, #523332</t>
+  </si>
+  <si>
+    <t>#0B2B51</t>
+  </si>
+  <si>
+    <t>#0B2B51, #0E3768, #124482, #16549E, #5B8EBA, #A5C7D0, #ECF2DD, #F9F0CD, #F2DAAF, #DEAA79, #C88F60, #AD7C54, #815F43, #614A38, #4C3D32</t>
+  </si>
+  <si>
+    <t>#F3E4C2</t>
+  </si>
+  <si>
+    <t>#061629</t>
+  </si>
+  <si>
+    <t>#0E3564, #D89B68, #815F43, #A5C7D0</t>
+  </si>
+  <si>
+    <t>#0081A7, #f07167, #A2E0CF, #FDE3C1</t>
+  </si>
+  <si>
+    <t>portal</t>
+  </si>
+  <si>
+    <t>#0D1B2A, #AF5D0F, #DEB77D, #354322</t>
+  </si>
+  <si>
+    <t>pem</t>
+  </si>
+  <si>
+    <t>#4C0C12</t>
+  </si>
+  <si>
+    <t>#1F1F1F</t>
+  </si>
+  <si>
+    <t>#FFFBEB</t>
+  </si>
+  <si>
+    <t>#112438, #342031, #571C2A, #7A1823, #992E2E, #B5604B, #D19168, #EDC385, #DBA563, #C98841, #B76B1F, #9C5710, #764C14, #504118, #2A361C</t>
   </si>
 </sst>
 </file>
@@ -206,9 +260,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,6 +751,75 @@
         <v>41</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Colors of current palette
</commit_message>
<xml_diff>
--- a/inst/data-raw/colors_table.xlsx
+++ b/inst/data-raw/colors_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentbagilet/Documents/Research/R_packages/mediocrethemes/inst/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF901244-EEA8-1C46-B2F3-BAB69795730F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D07526-B365-3B4A-BE49-BD0ED779CEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="15540" xr2:uid="{7AFE50BB-7247-734A-B3A5-BDA767197FA0}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
-    <t>color</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
@@ -222,6 +217,9 @@
   </si>
   <si>
     <t>#F07167</t>
+  </si>
+  <si>
+    <t>pal</t>
   </si>
 </sst>
 </file>
@@ -583,9 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D856B73-F7AB-7F4D-ABEA-B9947789DC7A}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -594,233 +590,233 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>